<commit_message>
Added Test 5 and 6
</commit_message>
<xml_diff>
--- a/Measurements/Test 2 - Chair obstacle/Statistics.xlsx
+++ b/Measurements/Test 2 - Chair obstacle/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\CodeFromGithub\SerialPortRead\Vamia-SerialPortReading\Measurements\Test 2 - Chair obstacle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B676F945-407F-40FE-B5A2-4B3C2BD07EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C225F57E-DA38-4BEE-9629-914F8CD3B0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5364" yWindow="552" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -834,61 +834,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>46.420599913279624</c:v>
+                  <c:v>45.121629908943603</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.441199826559249</c:v>
+                  <c:v>51.44325981788721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.963025007672869</c:v>
+                  <c:v>55.141176258056511</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.461799739838874</c:v>
+                  <c:v>57.764889726830816</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60.4</c:v>
+                  <c:v>59.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61.983624920952494</c:v>
+                  <c:v>61.462806167000117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>63.322560713564755</c:v>
+                  <c:v>62.868688749242992</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.482399653118492</c:v>
+                  <c:v>64.086519635774422</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>65.505450102066121</c:v>
+                  <c:v>65.160722607169419</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66.420599913279617</c:v>
+                  <c:v>66.121629908943603</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>68.004224834232119</c:v>
+                  <c:v>67.784436075943717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>69.34316062684438</c:v>
+                  <c:v>69.190318658186598</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>70.502999566398117</c:v>
+                  <c:v>70.408149544718015</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>71.526050015345746</c:v>
+                  <c:v>71.482352516113025</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>72.441199826559242</c:v>
+                  <c:v>72.44325981788721</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>73.269053529723749</c:v>
+                  <c:v>73.312506206209932</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>74.024824747511744</c:v>
+                  <c:v>74.106065984887323</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>74.72006687269598</c:v>
+                  <c:v>74.836070216330782</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>75.363760540124005</c:v>
+                  <c:v>75.511948567130204</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2269,10 +2269,10 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2587,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2601,10 +2601,10 @@
         <v>1</v>
       </c>
       <c r="F1">
-        <v>60.4</v>
+        <v>59.8</v>
       </c>
       <c r="G1">
-        <v>2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="F3">
         <f>10*$G$1*LOG(A3/100,10)+$F$1</f>
-        <v>46.420599913279624</v>
+        <v>45.121629908943603</v>
       </c>
       <c r="H3">
         <f>A3/100</f>
@@ -2644,7 +2644,7 @@
       </c>
       <c r="I3">
         <f>POWER(10, (B3-$F$1)/(10*$G$1))</f>
-        <v>0.48977881936844647</v>
+        <v>0.541169526546464</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F21" si="0">10*$G$1*LOG(A4/100,10)+$F$1</f>
-        <v>52.441199826559249</v>
+        <v>51.44325981788721</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H21" si="1">A4/100</f>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I21" si="2">POWER(10, (B4-$F$1)/(10*$G$1))</f>
-        <v>1.0964781961431855</v>
+        <v>1.1659144011798326</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2694,7 +2694,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>55.963025007672869</v>
+        <v>55.141176258056511</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
@@ -2702,7 +2702,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>1.4454397707459281</v>
+        <v>1.5168840366944534</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -2723,7 +2723,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>58.461799739838874</v>
+        <v>57.764889726830816</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>1.0964781961431855</v>
+        <v>1.1659144011798326</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>60.4</v>
+        <v>59.8</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.068000432514576</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2781,7 +2781,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>61.983624920952494</v>
+        <v>61.462806167000117</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>0.85113803820237666</v>
+        <v>0.91601959066105276</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>63.322560713564755</v>
+        <v>62.868688749242992</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>1.148153621496883</v>
+        <v>1.2181879120101162</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -2839,7 +2839,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>64.482399653118492</v>
+        <v>64.086519635774422</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>1.5488166189124821</v>
+        <v>1.6200328072641321</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>65.505450102066121</v>
+        <v>65.160722607169419</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>1.4454397707459281</v>
+        <v>1.5168840366944534</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2897,7 +2897,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>66.420599913279617</v>
+        <v>66.121629908943603</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
@@ -2905,7 +2905,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>1.7782794100389243</v>
+        <v>1.8478497974222927</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2926,7 +2926,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>68.004224834232119</v>
+        <v>67.784436075943717</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>3.7153522909717256</v>
+        <v>3.7275937203149403</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2955,7 +2955,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>69.34316062684438</v>
+        <v>69.190318658186598</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>3.8018939632056128</v>
+        <v>3.810240429946278</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2984,7 +2984,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>70.502999566398117</v>
+        <v>70.408149544718015</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>2.570395782768863</v>
+        <v>2.6245062966121004</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>71.526050015345746</v>
+        <v>71.482352516113025</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>2.3988329190194912</v>
+        <v>2.4574019042602622</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -3042,7 +3042,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>72.441199826559242</v>
+        <v>72.44325981788721</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>2.4547089156850319</v>
+        <v>2.5118864315095815</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>73.269053529723749</v>
+        <v>73.312506206209932</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
@@ -3079,7 +3079,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>3.8018939632056128</v>
+        <v>3.810240429946278</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>74.024824747511744</v>
+        <v>74.106065984887323</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>3.6307805477010127</v>
+        <v>3.6467396740964437</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>74.72006687269598</v>
+        <v>74.836070216330782</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>7.7624711662869235</v>
+        <v>7.5195261882835576</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -3158,7 +3158,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>75.363760540124005</v>
+        <v>75.511948567130204</v>
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>5.6234132519034956</v>
+        <v>5.5316811976172326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>